<commit_message>
Mise à jour des données et du graphique
</commit_message>
<xml_diff>
--- a/classement_youtube.xlsx
+++ b/classement_youtube.xlsx
@@ -489,7 +489,7 @@
         <v>45731.75537037037</v>
       </c>
       <c r="D2" t="n">
-        <v>6273</v>
+        <v>6312</v>
       </c>
       <c r="E2" t="n">
         <v>5635</v>
@@ -518,10 +518,10 @@
         <v>45731.65984953703</v>
       </c>
       <c r="D3" t="n">
-        <v>3939</v>
+        <v>4167</v>
       </c>
       <c r="E3" t="n">
-        <v>1302</v>
+        <v>1421</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -547,10 +547,10 @@
         <v>45731.65702546296</v>
       </c>
       <c r="D4" t="n">
-        <v>3323</v>
+        <v>3367</v>
       </c>
       <c r="E4" t="n">
-        <v>1292</v>
+        <v>1302</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
@@ -564,26 +564,26 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>hoA6ZAlniU4</t>
+          <t>5FjGLct9MQk</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Van&amp;Camp (Occitanie) - Célia Lauret</t>
+          <t>LuminyShop (Sud) - Michael Jeanmonod</t>
         </is>
       </c>
       <c r="C5" s="2" t="n">
-        <v>45731.73765046296</v>
+        <v>45731.67113425926</v>
       </c>
       <c r="D5" t="n">
-        <v>2242</v>
+        <v>3507</v>
       </c>
       <c r="E5" t="n">
-        <v>1192</v>
+        <v>1225</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=hoA6ZAlniU4</t>
+          <t>https://www.youtube.com/watch?v=5FjGLct9MQk</t>
         </is>
       </c>
       <c r="G5" t="n">
@@ -593,26 +593,26 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>5FjGLct9MQk</t>
+          <t>hoA6ZAlniU4</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>LuminyShop (Sud) - Michael Jeanmonod</t>
+          <t>Van&amp;Camp (Occitanie) - Célia Lauret</t>
         </is>
       </c>
       <c r="C6" s="2" t="n">
-        <v>45731.67113425926</v>
+        <v>45731.73765046296</v>
       </c>
       <c r="D6" t="n">
-        <v>3322</v>
+        <v>2257</v>
       </c>
       <c r="E6" t="n">
-        <v>1169</v>
+        <v>1192</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=5FjGLct9MQk</t>
+          <t>https://www.youtube.com/watch?v=hoA6ZAlniU4</t>
         </is>
       </c>
       <c r="G6" t="n">
@@ -634,10 +634,10 @@
         <v>45731.69415509259</v>
       </c>
       <c r="D7" t="n">
-        <v>5076</v>
+        <v>5097</v>
       </c>
       <c r="E7" t="n">
-        <v>1116</v>
+        <v>1117</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
@@ -663,10 +663,10 @@
         <v>45731.70519675926</v>
       </c>
       <c r="D8" t="n">
-        <v>1283</v>
+        <v>1447</v>
       </c>
       <c r="E8" t="n">
-        <v>822</v>
+        <v>1036</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
@@ -692,10 +692,10 @@
         <v>45731.78427083333</v>
       </c>
       <c r="D9" t="n">
-        <v>2650</v>
+        <v>2881</v>
       </c>
       <c r="E9" t="n">
-        <v>762</v>
+        <v>899</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
@@ -721,7 +721,7 @@
         <v>45731.74269675926</v>
       </c>
       <c r="D10" t="n">
-        <v>2120</v>
+        <v>2738</v>
       </c>
       <c r="E10" t="n">
         <v>762</v>
@@ -750,10 +750,10 @@
         <v>45731.68711805555</v>
       </c>
       <c r="D11" t="n">
-        <v>2169</v>
+        <v>2273</v>
       </c>
       <c r="E11" t="n">
-        <v>712</v>
+        <v>731</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
@@ -767,26 +767,26 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>BK1rMNeBrTQ</t>
+          <t>RentS8rqrpc</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Ozé (Sud) - Agathe Morandeau</t>
+          <t>Des Terres Minées (Ile-de-France) - Ayoub Kacemi</t>
         </is>
       </c>
       <c r="C12" s="2" t="n">
-        <v>45731.70387731482</v>
+        <v>45733.37125</v>
       </c>
       <c r="D12" t="n">
-        <v>2506</v>
+        <v>1726</v>
       </c>
       <c r="E12" t="n">
-        <v>685</v>
+        <v>708</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=BK1rMNeBrTQ</t>
+          <t>https://www.youtube.com/watch?v=RentS8rqrpc</t>
         </is>
       </c>
       <c r="G12" t="n">
@@ -796,26 +796,26 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>W5320T8taPo</t>
+          <t>BK1rMNeBrTQ</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>uplace (Auvergne-Rhône-Alpes) - Baptiste Menetrier</t>
+          <t>Ozé (Sud) - Agathe Morandeau</t>
         </is>
       </c>
       <c r="C13" s="2" t="n">
-        <v>45731.70635416666</v>
+        <v>45731.70387731482</v>
       </c>
       <c r="D13" t="n">
-        <v>2666</v>
+        <v>2545</v>
       </c>
       <c r="E13" t="n">
-        <v>651</v>
+        <v>688</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=W5320T8taPo</t>
+          <t>https://www.youtube.com/watch?v=BK1rMNeBrTQ</t>
         </is>
       </c>
       <c r="G13" t="n">
@@ -825,26 +825,26 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>8j84FmT0o7Y</t>
+          <t>W5320T8taPo</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Ajustable (Occitanie) - Justine Don</t>
+          <t>uplace (Auvergne-Rhône-Alpes) - Baptiste Menetrier</t>
         </is>
       </c>
       <c r="C14" s="2" t="n">
-        <v>45731.7728587963</v>
+        <v>45731.70635416666</v>
       </c>
       <c r="D14" t="n">
-        <v>2994</v>
+        <v>2731</v>
       </c>
       <c r="E14" t="n">
-        <v>474</v>
+        <v>668</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=8j84FmT0o7Y</t>
+          <t>https://www.youtube.com/watch?v=W5320T8taPo</t>
         </is>
       </c>
       <c r="G14" t="n">
@@ -854,26 +854,26 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>IU0ton7pf9c</t>
+          <t>8j84FmT0o7Y</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Disc'over (Provence-Alpes-Côte d’Azur) - Aurélien Boudon</t>
+          <t>Ajustable (Occitanie) - Justine Don</t>
         </is>
       </c>
       <c r="C15" s="2" t="n">
-        <v>45731.71851851852</v>
+        <v>45731.7728587963</v>
       </c>
       <c r="D15" t="n">
-        <v>2427</v>
+        <v>3026</v>
       </c>
       <c r="E15" t="n">
-        <v>450</v>
+        <v>476</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=IU0ton7pf9c</t>
+          <t>https://www.youtube.com/watch?v=8j84FmT0o7Y</t>
         </is>
       </c>
       <c r="G15" t="n">
@@ -883,26 +883,26 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>RentS8rqrpc</t>
+          <t>IU0ton7pf9c</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Des Terres Minées (Ile-de-France) - Ayoub Kacemi</t>
+          <t>Disc'over (Provence-Alpes-Côte d’Azur) - Aurélien Boudon</t>
         </is>
       </c>
       <c r="C16" s="2" t="n">
-        <v>45733.37125</v>
+        <v>45731.71851851852</v>
       </c>
       <c r="D16" t="n">
-        <v>1155</v>
+        <v>2463</v>
       </c>
       <c r="E16" t="n">
-        <v>435</v>
+        <v>456</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=RentS8rqrpc</t>
+          <t>https://www.youtube.com/watch?v=IU0ton7pf9c</t>
         </is>
       </c>
       <c r="G16" t="n">
@@ -924,10 +924,10 @@
         <v>45731.68974537037</v>
       </c>
       <c r="D17" t="n">
-        <v>1720</v>
+        <v>1730</v>
       </c>
       <c r="E17" t="n">
-        <v>426</v>
+        <v>453</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
@@ -953,10 +953,10 @@
         <v>45731.69576388889</v>
       </c>
       <c r="D18" t="n">
-        <v>1444</v>
+        <v>1452</v>
       </c>
       <c r="E18" t="n">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
@@ -982,10 +982,10 @@
         <v>45731.71129629629</v>
       </c>
       <c r="D19" t="n">
-        <v>2369</v>
+        <v>2441</v>
       </c>
       <c r="E19" t="n">
-        <v>370</v>
+        <v>375</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
@@ -1011,10 +1011,10 @@
         <v>45731.72594907408</v>
       </c>
       <c r="D20" t="n">
-        <v>1464</v>
+        <v>1479</v>
       </c>
       <c r="E20" t="n">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
@@ -1040,10 +1040,10 @@
         <v>45734.71620370371</v>
       </c>
       <c r="D21" t="n">
-        <v>1294</v>
+        <v>1324</v>
       </c>
       <c r="E21" t="n">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
@@ -1069,7 +1069,7 @@
         <v>45731.66652777778</v>
       </c>
       <c r="D22" t="n">
-        <v>1211</v>
+        <v>1218</v>
       </c>
       <c r="E22" t="n">
         <v>328</v>
@@ -1098,10 +1098,10 @@
         <v>45731.67795138889</v>
       </c>
       <c r="D23" t="n">
-        <v>1259</v>
+        <v>1308</v>
       </c>
       <c r="E23" t="n">
-        <v>322</v>
+        <v>327</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
@@ -1127,10 +1127,10 @@
         <v>45731.74208333333</v>
       </c>
       <c r="D24" t="n">
-        <v>1996</v>
+        <v>2019</v>
       </c>
       <c r="E24" t="n">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
@@ -1156,10 +1156,10 @@
         <v>45731.746875</v>
       </c>
       <c r="D25" t="n">
-        <v>1111</v>
+        <v>1121</v>
       </c>
       <c r="E25" t="n">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="F25" t="inlineStr">
         <is>
@@ -1185,10 +1185,10 @@
         <v>45734.46524305556</v>
       </c>
       <c r="D26" t="n">
-        <v>1918</v>
+        <v>2019</v>
       </c>
       <c r="E26" t="n">
-        <v>272</v>
+        <v>285</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>
@@ -1214,10 +1214,10 @@
         <v>45731.66978009259</v>
       </c>
       <c r="D27" t="n">
-        <v>1038</v>
+        <v>1051</v>
       </c>
       <c r="E27" t="n">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>
@@ -1231,26 +1231,26 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>KhWwd2xcKmo</t>
+          <t>uYv_In2beXM</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>alchemys (Ile de France) - Lucas Barbosa</t>
+          <t>HUZOG INDUSTRTY (Normandie) - Aubin Rahmani</t>
         </is>
       </c>
       <c r="C28" s="2" t="n">
-        <v>45731.71417824074</v>
+        <v>45732.61858796296</v>
       </c>
       <c r="D28" t="n">
-        <v>1255</v>
+        <v>1083</v>
       </c>
       <c r="E28" t="n">
         <v>242</v>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=KhWwd2xcKmo</t>
+          <t>https://www.youtube.com/watch?v=uYv_In2beXM</t>
         </is>
       </c>
       <c r="G28" t="n">
@@ -1260,26 +1260,26 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2QpaqiU0DDE</t>
+          <t>KhWwd2xcKmo</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>SAVOTEY (Auvergne-Rhône-Alpes) - Sarine Chau</t>
+          <t>alchemys (Ile de France) - Lucas Barbosa</t>
         </is>
       </c>
       <c r="C29" s="2" t="n">
-        <v>45732.61717592592</v>
+        <v>45731.71417824074</v>
       </c>
       <c r="D29" t="n">
-        <v>1628</v>
+        <v>1261</v>
       </c>
       <c r="E29" t="n">
-        <v>237</v>
+        <v>242</v>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=2QpaqiU0DDE</t>
+          <t>https://www.youtube.com/watch?v=KhWwd2xcKmo</t>
         </is>
       </c>
       <c r="G29" t="n">
@@ -1289,26 +1289,26 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>i-Dg1ig8tuc</t>
+          <t>2QpaqiU0DDE</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>COME PRIMA (Grand Est) - Fanny Barro</t>
+          <t>SAVOTEY (Auvergne-Rhône-Alpes) - Sarine Chau</t>
         </is>
       </c>
       <c r="C30" s="2" t="n">
-        <v>45731.74027777778</v>
+        <v>45732.61717592592</v>
       </c>
       <c r="D30" t="n">
-        <v>1533</v>
+        <v>1653</v>
       </c>
       <c r="E30" t="n">
-        <v>233</v>
+        <v>239</v>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=i-Dg1ig8tuc</t>
+          <t>https://www.youtube.com/watch?v=2QpaqiU0DDE</t>
         </is>
       </c>
       <c r="G30" t="n">
@@ -1318,26 +1318,26 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>yvU0_Z5V8xY</t>
+          <t>i-Dg1ig8tuc</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>No Plane To Go  (Ile de France) -  Lucie Cossia</t>
+          <t>COME PRIMA (Grand Est) - Fanny Barro</t>
         </is>
       </c>
       <c r="C31" s="2" t="n">
-        <v>45731.75700231481</v>
+        <v>45731.74027777778</v>
       </c>
       <c r="D31" t="n">
-        <v>511</v>
+        <v>1548</v>
       </c>
       <c r="E31" t="n">
-        <v>219</v>
+        <v>233</v>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=yvU0_Z5V8xY</t>
+          <t>https://www.youtube.com/watch?v=i-Dg1ig8tuc</t>
         </is>
       </c>
       <c r="G31" t="n">
@@ -1347,26 +1347,26 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>uYv_In2beXM</t>
+          <t>yvU0_Z5V8xY</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>HUZOG INDUSTRTY (Normandie) - Aubin Rahmani</t>
+          <t>No Plane To Go  (Ile de France) -  Lucie Cossia</t>
         </is>
       </c>
       <c r="C32" s="2" t="n">
-        <v>45732.61858796296</v>
+        <v>45731.75700231481</v>
       </c>
       <c r="D32" t="n">
-        <v>973</v>
+        <v>522</v>
       </c>
       <c r="E32" t="n">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=uYv_In2beXM</t>
+          <t>https://www.youtube.com/watch?v=yvU0_Z5V8xY</t>
         </is>
       </c>
       <c r="G32" t="n">
@@ -1388,10 +1388,10 @@
         <v>45731.69851851852</v>
       </c>
       <c r="D33" t="n">
-        <v>880</v>
+        <v>890</v>
       </c>
       <c r="E33" t="n">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="F33" t="inlineStr">
         <is>
@@ -1417,10 +1417,10 @@
         <v>45731.77814814815</v>
       </c>
       <c r="D34" t="n">
-        <v>859</v>
+        <v>871</v>
       </c>
       <c r="E34" t="n">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="F34" t="inlineStr">
         <is>
@@ -1434,26 +1434,26 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>w4_H7lnDxHw</t>
+          <t>ak7VnMRovWc</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Revisité Ile-de-France) - Anne Gulino</t>
+          <t>Primaire (Grand Est) - Lucie Le May</t>
         </is>
       </c>
       <c r="C35" s="2" t="n">
-        <v>45731.71700231481</v>
+        <v>45731.7528587963</v>
       </c>
       <c r="D35" t="n">
-        <v>579</v>
+        <v>869</v>
       </c>
       <c r="E35" t="n">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=w4_H7lnDxHw</t>
+          <t>https://www.youtube.com/watch?v=ak7VnMRovWc</t>
         </is>
       </c>
       <c r="G35" t="n">
@@ -1463,26 +1463,26 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Lgb9olWKkBg</t>
+          <t>w4_H7lnDxHw</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Ride Enjoy (Pays de la Loire) - Léo Gentilhomme</t>
+          <t>Revisité Ile-de-France) - Anne Gulino</t>
         </is>
       </c>
       <c r="C36" s="2" t="n">
-        <v>45731.69020833333</v>
+        <v>45731.71700231481</v>
       </c>
       <c r="D36" t="n">
-        <v>1124</v>
+        <v>582</v>
       </c>
       <c r="E36" t="n">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=Lgb9olWKkBg</t>
+          <t>https://www.youtube.com/watch?v=w4_H7lnDxHw</t>
         </is>
       </c>
       <c r="G36" t="n">
@@ -1492,26 +1492,26 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>ak7VnMRovWc</t>
+          <t>Lgb9olWKkBg</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Primaire (Grand Est) - Lucie Le May</t>
+          <t>Ride Enjoy (Pays de la Loire) - Léo Gentilhomme</t>
         </is>
       </c>
       <c r="C37" s="2" t="n">
-        <v>45731.7528587963</v>
+        <v>45731.69020833333</v>
       </c>
       <c r="D37" t="n">
-        <v>852</v>
+        <v>1130</v>
       </c>
       <c r="E37" t="n">
         <v>162</v>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=ak7VnMRovWc</t>
+          <t>https://www.youtube.com/watch?v=Lgb9olWKkBg</t>
         </is>
       </c>
       <c r="G37" t="n">
@@ -1533,10 +1533,10 @@
         <v>45731.70513888889</v>
       </c>
       <c r="D38" t="n">
-        <v>477</v>
+        <v>481</v>
       </c>
       <c r="E38" t="n">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="F38" t="inlineStr">
         <is>
@@ -1562,10 +1562,10 @@
         <v>45731.73831018519</v>
       </c>
       <c r="D39" t="n">
-        <v>821</v>
+        <v>832</v>
       </c>
       <c r="E39" t="n">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="F39" t="inlineStr">
         <is>
@@ -1579,26 +1579,26 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>93Y9MBzG_ck</t>
+          <t>mOqYITDsIFM</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Hnyn (Ile-de-France) - Heranne Excellent</t>
+          <t>ZePowerNet (Grand Est) - Mamadou Misbaou Barry</t>
         </is>
       </c>
       <c r="C40" s="2" t="n">
-        <v>45731.66284722222</v>
+        <v>45731.73930555556</v>
       </c>
       <c r="D40" t="n">
-        <v>976</v>
+        <v>666</v>
       </c>
       <c r="E40" t="n">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=93Y9MBzG_ck</t>
+          <t>https://www.youtube.com/watch?v=mOqYITDsIFM</t>
         </is>
       </c>
       <c r="G40" t="n">
@@ -1608,26 +1608,26 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>mOqYITDsIFM</t>
+          <t>i9e-beHIxJo</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>ZePowerNet (Grand Est) - Mamadou Misbaou Barry</t>
+          <t>Handépassement (Ile de France) - Myriam Hakem</t>
         </is>
       </c>
       <c r="C41" s="2" t="n">
-        <v>45731.73930555556</v>
+        <v>45731.67952546296</v>
       </c>
       <c r="D41" t="n">
-        <v>633</v>
+        <v>966</v>
       </c>
       <c r="E41" t="n">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=mOqYITDsIFM</t>
+          <t>https://www.youtube.com/watch?v=i9e-beHIxJo</t>
         </is>
       </c>
       <c r="G41" t="n">
@@ -1637,26 +1637,26 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>i9e-beHIxJo</t>
+          <t>93Y9MBzG_ck</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Handépassement (Ile de France) - Myriam Hakem</t>
+          <t>Hnyn (Ile-de-France) - Heranne Excellent</t>
         </is>
       </c>
       <c r="C42" s="2" t="n">
-        <v>45731.67952546296</v>
+        <v>45731.66284722222</v>
       </c>
       <c r="D42" t="n">
-        <v>940</v>
+        <v>982</v>
       </c>
       <c r="E42" t="n">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=i9e-beHIxJo</t>
+          <t>https://www.youtube.com/watch?v=93Y9MBzG_ck</t>
         </is>
       </c>
       <c r="G42" t="n">
@@ -1666,26 +1666,26 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>zXXvFS4S4UM</t>
+          <t>eexQ8l-Cqgc</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Cclean (Ile de France) - Cécilia KWAKWA</t>
+          <t>S W A G  Studio (Provence-Alpes-Côte d'Azur) -  Pauline Terestchenko</t>
         </is>
       </c>
       <c r="C43" s="2" t="n">
-        <v>45732.65084490741</v>
+        <v>45731.72136574074</v>
       </c>
       <c r="D43" t="n">
-        <v>638</v>
+        <v>364</v>
       </c>
       <c r="E43" t="n">
-        <v>131</v>
+        <v>143</v>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=zXXvFS4S4UM</t>
+          <t>https://www.youtube.com/watch?v=eexQ8l-Cqgc</t>
         </is>
       </c>
       <c r="G43" t="n">
@@ -1695,26 +1695,26 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>eexQ8l-Cqgc</t>
+          <t>zXXvFS4S4UM</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>S W A G  Studio (Provence-Alpes-Côte d'Azur) -  Pauline Terestchenko</t>
+          <t>Cclean (Ile de France) - Cécilia KWAKWA</t>
         </is>
       </c>
       <c r="C44" s="2" t="n">
-        <v>45731.72136574074</v>
+        <v>45732.65084490741</v>
       </c>
       <c r="D44" t="n">
-        <v>242</v>
+        <v>661</v>
       </c>
       <c r="E44" t="n">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=eexQ8l-Cqgc</t>
+          <t>https://www.youtube.com/watch?v=zXXvFS4S4UM</t>
         </is>
       </c>
       <c r="G44" t="n">
@@ -1736,10 +1736,10 @@
         <v>45731.65853009259</v>
       </c>
       <c r="D45" t="n">
-        <v>791</v>
+        <v>803</v>
       </c>
       <c r="E45" t="n">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F45" t="inlineStr">
         <is>
@@ -1765,10 +1765,10 @@
         <v>45731.76277777777</v>
       </c>
       <c r="D46" t="n">
-        <v>1226</v>
+        <v>1248</v>
       </c>
       <c r="E46" t="n">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F46" t="inlineStr">
         <is>
@@ -1782,26 +1782,26 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>fmAEjSzgWBU</t>
+          <t>Cqelo17KW68</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Drive Lady (Normandie) - Camille Cottard</t>
+          <t>My kitchen (Ile-de-France) - Céline BUDAK</t>
         </is>
       </c>
       <c r="C47" s="2" t="n">
-        <v>45731.69076388889</v>
+        <v>45733.4946875</v>
       </c>
       <c r="D47" t="n">
-        <v>464</v>
+        <v>1244</v>
       </c>
       <c r="E47" t="n">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=fmAEjSzgWBU</t>
+          <t>https://www.youtube.com/watch?v=Cqelo17KW68</t>
         </is>
       </c>
       <c r="G47" t="n">
@@ -1811,26 +1811,26 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Cqelo17KW68</t>
+          <t>fmAEjSzgWBU</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>My kitchen (Ile-de-France) - Céline BUDAK</t>
+          <t>Drive Lady (Normandie) - Camille Cottard</t>
         </is>
       </c>
       <c r="C48" s="2" t="n">
-        <v>45733.4946875</v>
+        <v>45731.69076388889</v>
       </c>
       <c r="D48" t="n">
-        <v>1208</v>
+        <v>466</v>
       </c>
       <c r="E48" t="n">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=Cqelo17KW68</t>
+          <t>https://www.youtube.com/watch?v=fmAEjSzgWBU</t>
         </is>
       </c>
       <c r="G48" t="n">
@@ -1852,7 +1852,7 @@
         <v>45732.61524305555</v>
       </c>
       <c r="D49" t="n">
-        <v>829</v>
+        <v>846</v>
       </c>
       <c r="E49" t="n">
         <v>91</v>
@@ -1881,10 +1881,10 @@
         <v>45732.61957175926</v>
       </c>
       <c r="D50" t="n">
-        <v>599</v>
+        <v>617</v>
       </c>
       <c r="E50" t="n">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F50" t="inlineStr">
         <is>
@@ -1910,7 +1910,7 @@
         <v>45731.74450231482</v>
       </c>
       <c r="D51" t="n">
-        <v>610</v>
+        <v>617</v>
       </c>
       <c r="E51" t="n">
         <v>86</v>
@@ -1939,10 +1939,10 @@
         <v>45731.73282407408</v>
       </c>
       <c r="D52" t="n">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="E52" t="n">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F52" t="inlineStr">
         <is>
@@ -1968,10 +1968,10 @@
         <v>45732.63519675926</v>
       </c>
       <c r="D53" t="n">
-        <v>590</v>
+        <v>605</v>
       </c>
       <c r="E53" t="n">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F53" t="inlineStr">
         <is>
@@ -1985,26 +1985,26 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>I0a13hzust4</t>
+          <t>mSziXZIgVKw</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Anbizioa (Nouvelle Aquitaine) - Marine Durand</t>
+          <t>Kam e leon (Nouvelle Aquitaine) - Eden Rouvreau</t>
         </is>
       </c>
       <c r="C54" s="2" t="n">
-        <v>45731.69967592593</v>
+        <v>45731.74932870371</v>
       </c>
       <c r="D54" t="n">
-        <v>361</v>
+        <v>410</v>
       </c>
       <c r="E54" t="n">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=I0a13hzust4</t>
+          <t>https://www.youtube.com/watch?v=mSziXZIgVKw</t>
         </is>
       </c>
       <c r="G54" t="n">
@@ -2014,26 +2014,26 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>mSziXZIgVKw</t>
+          <t>I0a13hzust4</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Kam e leon (Nouvelle Aquitaine) - Eden Rouvreau</t>
+          <t>Anbizioa (Nouvelle Aquitaine) - Marine Durand</t>
         </is>
       </c>
       <c r="C55" s="2" t="n">
-        <v>45731.74932870371</v>
+        <v>45731.69967592593</v>
       </c>
       <c r="D55" t="n">
-        <v>401</v>
+        <v>364</v>
       </c>
       <c r="E55" t="n">
         <v>67</v>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=mSziXZIgVKw</t>
+          <t>https://www.youtube.com/watch?v=I0a13hzust4</t>
         </is>
       </c>
       <c r="G55" t="n">
@@ -2055,7 +2055,7 @@
         <v>45731.72815972222</v>
       </c>
       <c r="D56" t="n">
-        <v>311</v>
+        <v>316</v>
       </c>
       <c r="E56" t="n">
         <v>60</v>
@@ -2084,10 +2084,10 @@
         <v>45731.75552083334</v>
       </c>
       <c r="D57" t="n">
-        <v>249</v>
+        <v>255</v>
       </c>
       <c r="E57" t="n">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F57" t="inlineStr">
         <is>
@@ -2113,7 +2113,7 @@
         <v>45731.75940972222</v>
       </c>
       <c r="D58" t="n">
-        <v>312</v>
+        <v>324</v>
       </c>
       <c r="E58" t="n">
         <v>53</v>
@@ -2142,10 +2142,10 @@
         <v>45732.56851851852</v>
       </c>
       <c r="D59" t="n">
-        <v>511</v>
+        <v>523</v>
       </c>
       <c r="E59" t="n">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F59" t="inlineStr">
         <is>
@@ -2171,10 +2171,10 @@
         <v>45731.73631944445</v>
       </c>
       <c r="D60" t="n">
-        <v>461</v>
+        <v>475</v>
       </c>
       <c r="E60" t="n">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F60" t="inlineStr">
         <is>
@@ -2200,10 +2200,10 @@
         <v>45731.74563657407</v>
       </c>
       <c r="D61" t="n">
-        <v>258</v>
+        <v>265</v>
       </c>
       <c r="E61" t="n">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F61" t="inlineStr">
         <is>
@@ -2217,26 +2217,26 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>s33dV36tMJg</t>
+          <t>K4imLcfYffQ</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Aux ptits zouzous  (Auvergne Rhône Alpes) - Kimberly Simonet</t>
+          <t>SOUM SOUM (Auvergne-Rhône-Alpes) - Ismaël Ailane</t>
         </is>
       </c>
       <c r="C62" s="2" t="n">
-        <v>45731.66840277778</v>
+        <v>45732.60997685185</v>
       </c>
       <c r="D62" t="n">
-        <v>905</v>
+        <v>901</v>
       </c>
       <c r="E62" t="n">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=s33dV36tMJg</t>
+          <t>https://www.youtube.com/watch?v=K4imLcfYffQ</t>
         </is>
       </c>
       <c r="G62" t="n">
@@ -2258,10 +2258,10 @@
         <v>45734.61689814815</v>
       </c>
       <c r="D63" t="n">
-        <v>432</v>
+        <v>455</v>
       </c>
       <c r="E63" t="n">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="F63" t="inlineStr">
         <is>
@@ -2275,26 +2275,26 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>K4imLcfYffQ</t>
+          <t>s33dV36tMJg</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>SOUM SOUM (Auvergne-Rhône-Alpes) - Ismaël Ailane</t>
+          <t>Aux ptits zouzous  (Auvergne Rhône Alpes) - Kimberly Simonet</t>
         </is>
       </c>
       <c r="C64" s="2" t="n">
-        <v>45732.60997685185</v>
+        <v>45731.66840277778</v>
       </c>
       <c r="D64" t="n">
-        <v>886</v>
+        <v>920</v>
       </c>
       <c r="E64" t="n">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=K4imLcfYffQ</t>
+          <t>https://www.youtube.com/watch?v=s33dV36tMJg</t>
         </is>
       </c>
       <c r="G64" t="n">
@@ -2316,7 +2316,7 @@
         <v>45731.69471064815</v>
       </c>
       <c r="D65" t="n">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="E65" t="n">
         <v>42</v>
@@ -2345,7 +2345,7 @@
         <v>45731.70770833334</v>
       </c>
       <c r="D66" t="n">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="E66" t="n">
         <v>41</v>
@@ -2362,26 +2362,26 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>HhN8skozWWM</t>
+          <t>OVg1lgo34ng</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Hyppalektryon (Hauts-de-France) - Elisa Douchez</t>
+          <t>Mikoo (Provence-Alpes-Côte d’Azur) - Lucas Cuordifede</t>
         </is>
       </c>
       <c r="C67" s="2" t="n">
-        <v>45731.73899305556</v>
+        <v>45732.88743055556</v>
       </c>
       <c r="D67" t="n">
-        <v>238</v>
+        <v>414</v>
       </c>
       <c r="E67" t="n">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=HhN8skozWWM</t>
+          <t>https://www.youtube.com/watch?v=OVg1lgo34ng</t>
         </is>
       </c>
       <c r="G67" t="n">
@@ -2391,26 +2391,26 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>OVg1lgo34ng</t>
+          <t>HhN8skozWWM</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Mikoo (Provence-Alpes-Côte d’Azur) - Lucas Cuordifede</t>
+          <t>Hyppalektryon (Hauts-de-France) - Elisa Douchez</t>
         </is>
       </c>
       <c r="C68" s="2" t="n">
-        <v>45732.88743055556</v>
+        <v>45731.73899305556</v>
       </c>
       <c r="D68" t="n">
-        <v>399</v>
+        <v>246</v>
       </c>
       <c r="E68" t="n">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=OVg1lgo34ng</t>
+          <t>https://www.youtube.com/watch?v=HhN8skozWWM</t>
         </is>
       </c>
       <c r="G68" t="n">
@@ -2432,10 +2432,10 @@
         <v>45731.73412037037</v>
       </c>
       <c r="D69" t="n">
-        <v>201</v>
+        <v>210</v>
       </c>
       <c r="E69" t="n">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F69" t="inlineStr">
         <is>
@@ -2449,26 +2449,26 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>ZeI4HS5sEzM</t>
+          <t>TFryzA55HpI</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Le Spark (Grand Est) - Aurélien Defontenay</t>
+          <t>Lueurs d'antan (Bretagne) - Axelle Trouillet</t>
         </is>
       </c>
       <c r="C70" s="2" t="n">
-        <v>45731.69685185186</v>
+        <v>45732.62079861111</v>
       </c>
       <c r="D70" t="n">
-        <v>168</v>
+        <v>238</v>
       </c>
       <c r="E70" t="n">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=ZeI4HS5sEzM</t>
+          <t>https://www.youtube.com/watch?v=TFryzA55HpI</t>
         </is>
       </c>
       <c r="G70" t="n">
@@ -2478,26 +2478,26 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>ye-XF2r7mvU</t>
+          <t>ZeI4HS5sEzM</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Dokamy (Nouvelle Aquitaine) -  Margaux Deshayes</t>
+          <t>Le Spark (Grand Est) - Aurélien Defontenay</t>
         </is>
       </c>
       <c r="C71" s="2" t="n">
-        <v>45731.68137731482</v>
+        <v>45731.69685185186</v>
       </c>
       <c r="D71" t="n">
-        <v>211</v>
+        <v>170</v>
       </c>
       <c r="E71" t="n">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=ye-XF2r7mvU</t>
+          <t>https://www.youtube.com/watch?v=ZeI4HS5sEzM</t>
         </is>
       </c>
       <c r="G71" t="n">
@@ -2519,10 +2519,10 @@
         <v>45731.77892361111</v>
       </c>
       <c r="D72" t="n">
-        <v>205</v>
+        <v>219</v>
       </c>
       <c r="E72" t="n">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F72" t="inlineStr">
         <is>
@@ -2536,26 +2536,26 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>TFryzA55HpI</t>
+          <t>ye-XF2r7mvU</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Lueurs d'antan (Bretagne) - Axelle Trouillet</t>
+          <t>Dokamy (Nouvelle Aquitaine) -  Margaux Deshayes</t>
         </is>
       </c>
       <c r="C73" s="2" t="n">
-        <v>45732.62079861111</v>
+        <v>45731.68137731482</v>
       </c>
       <c r="D73" t="n">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="E73" t="n">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=TFryzA55HpI</t>
+          <t>https://www.youtube.com/watch?v=ye-XF2r7mvU</t>
         </is>
       </c>
       <c r="G73" t="n">
@@ -2565,26 +2565,26 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>ck9GYOQkEUs</t>
+          <t>Ax4rhyVKP2c</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>P'tit Loup (Grand Est) - Léa Sabatier</t>
+          <t>MonCoachDePoche (Grand Est) - Lucas Gerum</t>
         </is>
       </c>
       <c r="C74" s="2" t="n">
-        <v>45731.67600694444</v>
+        <v>45731.69309027777</v>
       </c>
       <c r="D74" t="n">
-        <v>236</v>
+        <v>249</v>
       </c>
       <c r="E74" t="n">
         <v>22</v>
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=ck9GYOQkEUs</t>
+          <t>https://www.youtube.com/watch?v=Ax4rhyVKP2c</t>
         </is>
       </c>
       <c r="G74" t="n">
@@ -2594,26 +2594,26 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Ax4rhyVKP2c</t>
+          <t>ck9GYOQkEUs</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>MonCoachDePoche (Grand Est) - Lucas Gerum</t>
+          <t>P'tit Loup (Grand Est) - Léa Sabatier</t>
         </is>
       </c>
       <c r="C75" s="2" t="n">
-        <v>45731.69309027777</v>
+        <v>45731.67600694444</v>
       </c>
       <c r="D75" t="n">
-        <v>246</v>
+        <v>236</v>
       </c>
       <c r="E75" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=Ax4rhyVKP2c</t>
+          <t>https://www.youtube.com/watch?v=ck9GYOQkEUs</t>
         </is>
       </c>
       <c r="G75" t="n">
@@ -2635,10 +2635,10 @@
         <v>45731.71251157407</v>
       </c>
       <c r="D76" t="n">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="E76" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F76" t="inlineStr">
         <is>
@@ -2652,26 +2652,26 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>wpgkQPfjecA</t>
+          <t>tirkNG6e8bU</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Martin Stein Solutions (Ile de France) - Nicolas Lobstein</t>
+          <t>The Magic Coffee (Hauts-de-France) - Inasse Toumi</t>
         </is>
       </c>
       <c r="C77" s="2" t="n">
-        <v>45731.75690972222</v>
+        <v>45732.62953703704</v>
       </c>
       <c r="D77" t="n">
-        <v>146</v>
+        <v>181</v>
       </c>
       <c r="E77" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=wpgkQPfjecA</t>
+          <t>https://www.youtube.com/watch?v=tirkNG6e8bU</t>
         </is>
       </c>
       <c r="G77" t="n">
@@ -2681,26 +2681,26 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>tirkNG6e8bU</t>
+          <t>wpgkQPfjecA</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>The Magic Coffee (Hauts-de-France) - Inasse Toumi</t>
+          <t>Martin Stein Solutions (Ile de France) - Nicolas Lobstein</t>
         </is>
       </c>
       <c r="C78" s="2" t="n">
-        <v>45732.62953703704</v>
+        <v>45731.75690972222</v>
       </c>
       <c r="D78" t="n">
-        <v>169</v>
+        <v>153</v>
       </c>
       <c r="E78" t="n">
         <v>19</v>
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=tirkNG6e8bU</t>
+          <t>https://www.youtube.com/watch?v=wpgkQPfjecA</t>
         </is>
       </c>
       <c r="G78" t="n">
@@ -2722,7 +2722,7 @@
         <v>45731.68836805555</v>
       </c>
       <c r="D79" t="n">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="E79" t="n">
         <v>19</v>
@@ -2751,10 +2751,10 @@
         <v>45731.75413194444</v>
       </c>
       <c r="D80" t="n">
-        <v>186</v>
+        <v>193</v>
       </c>
       <c r="E80" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F80" t="inlineStr">
         <is>
@@ -2768,26 +2768,26 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>zjNk_GBOz-U</t>
+          <t>DR_P7zvNs3Y</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Les Harmonieuses (Ile de France) - Elodie Te</t>
+          <t>NoteHear (Occitanie) - Nazarii Ivakhniuk</t>
         </is>
       </c>
       <c r="C81" s="2" t="n">
-        <v>45731.7478587963</v>
+        <v>45735.49681712963</v>
       </c>
       <c r="D81" t="n">
-        <v>122</v>
+        <v>412</v>
       </c>
       <c r="E81" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=zjNk_GBOz-U</t>
+          <t>https://www.youtube.com/watch?v=DR_P7zvNs3Y</t>
         </is>
       </c>
       <c r="G81" t="n">
@@ -2797,26 +2797,26 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>DR_P7zvNs3Y</t>
+          <t>zjNk_GBOz-U</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>NoteHear (Occitanie) - Nazarii Ivakhniuk</t>
+          <t>Les Harmonieuses (Ile de France) - Elodie Te</t>
         </is>
       </c>
       <c r="C82" s="2" t="n">
-        <v>45735.49681712963</v>
+        <v>45731.7478587963</v>
       </c>
       <c r="D82" t="n">
-        <v>384</v>
+        <v>130</v>
       </c>
       <c r="E82" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=DR_P7zvNs3Y</t>
+          <t>https://www.youtube.com/watch?v=zjNk_GBOz-U</t>
         </is>
       </c>
       <c r="G82" t="n">
@@ -2826,26 +2826,26 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>8u2qC29LxPE</t>
+          <t>l11oYhr0tX8</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>La Repousse (Grand Est) - Viktor Macé</t>
+          <t>MindCare (Ile-de-France) - Djenaba Toure</t>
         </is>
       </c>
       <c r="C83" s="2" t="n">
-        <v>45736.40002314815</v>
+        <v>45732.58172453703</v>
       </c>
       <c r="D83" t="n">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="E83" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=8u2qC29LxPE</t>
+          <t>https://www.youtube.com/watch?v=l11oYhr0tX8</t>
         </is>
       </c>
       <c r="G83" t="n">
@@ -2855,26 +2855,26 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>YxsHa3ivN3k</t>
+          <t>8u2qC29LxPE</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Caelum (Occitanie) - Juan Carlos Guzman</t>
+          <t>La Repousse (Grand Est) - Viktor Macé</t>
         </is>
       </c>
       <c r="C84" s="2" t="n">
-        <v>45732.57215277778</v>
+        <v>45736.40002314815</v>
       </c>
       <c r="D84" t="n">
-        <v>149</v>
+        <v>214</v>
       </c>
       <c r="E84" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=YxsHa3ivN3k</t>
+          <t>https://www.youtube.com/watch?v=8u2qC29LxPE</t>
         </is>
       </c>
       <c r="G84" t="n">
@@ -2896,10 +2896,10 @@
         <v>45732.58274305556</v>
       </c>
       <c r="D85" t="n">
-        <v>88</v>
+        <v>103</v>
       </c>
       <c r="E85" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F85" t="inlineStr">
         <is>
@@ -2913,26 +2913,26 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>l11oYhr0tX8</t>
+          <t>YxsHa3ivN3k</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>MindCare (Ile-de-France) - Djenaba Toure</t>
+          <t>Caelum (Occitanie) - Juan Carlos Guzman</t>
         </is>
       </c>
       <c r="C86" s="2" t="n">
-        <v>45732.58172453703</v>
+        <v>45732.57215277778</v>
       </c>
       <c r="D86" t="n">
-        <v>99</v>
+        <v>160</v>
       </c>
       <c r="E86" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=l11oYhr0tX8</t>
+          <t>https://www.youtube.com/watch?v=YxsHa3ivN3k</t>
         </is>
       </c>
       <c r="G86" t="n">
@@ -2942,26 +2942,26 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>aYu9Ch98gSM</t>
+          <t>OdOQeUkmwSE</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>Mosaic (Ile de France) -Antoine Robin</t>
+          <t>Indup (Ile de France) - Emrys Djebbari</t>
         </is>
       </c>
       <c r="C87" s="2" t="n">
-        <v>45731.76017361111</v>
+        <v>45731.67466435185</v>
       </c>
       <c r="D87" t="n">
-        <v>125</v>
+        <v>408</v>
       </c>
       <c r="E87" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=aYu9Ch98gSM</t>
+          <t>https://www.youtube.com/watch?v=OdOQeUkmwSE</t>
         </is>
       </c>
       <c r="G87" t="n">
@@ -2971,26 +2971,26 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>OdOQeUkmwSE</t>
+          <t>yERDv4dSrVQ</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>Indup (Ile de France) - Emrys Djebbari</t>
+          <t>UBCE SAS (Ile de France) - Céline Li</t>
         </is>
       </c>
       <c r="C88" s="2" t="n">
-        <v>45731.67466435185</v>
+        <v>45731.75136574074</v>
       </c>
       <c r="D88" t="n">
-        <v>403</v>
+        <v>140</v>
       </c>
       <c r="E88" t="n">
         <v>6</v>
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=OdOQeUkmwSE</t>
+          <t>https://www.youtube.com/watch?v=yERDv4dSrVQ</t>
         </is>
       </c>
       <c r="G88" t="n">
@@ -3000,26 +3000,26 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>y7Pa-9pa0nA</t>
+          <t>aYu9Ch98gSM</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Sweefy (Auvergne Rhône Alpes) - Jonathan Godefroid</t>
+          <t>Mosaic (Ile de France) -Antoine Robin</t>
         </is>
       </c>
       <c r="C89" s="2" t="n">
-        <v>45731.69703703704</v>
+        <v>45731.76017361111</v>
       </c>
       <c r="D89" t="n">
-        <v>80</v>
+        <v>132</v>
       </c>
       <c r="E89" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=y7Pa-9pa0nA</t>
+          <t>https://www.youtube.com/watch?v=aYu9Ch98gSM</t>
         </is>
       </c>
       <c r="G89" t="n">
@@ -3029,26 +3029,26 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>yERDv4dSrVQ</t>
+          <t>y7Pa-9pa0nA</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>UBCE SAS (Ile de France) - Céline Li</t>
+          <t>Sweefy (Auvergne Rhône Alpes) - Jonathan Godefroid</t>
         </is>
       </c>
       <c r="C90" s="2" t="n">
-        <v>45731.75136574074</v>
+        <v>45731.69703703704</v>
       </c>
       <c r="D90" t="n">
-        <v>134</v>
+        <v>82</v>
       </c>
       <c r="E90" t="n">
         <v>5</v>
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=yERDv4dSrVQ</t>
+          <t>https://www.youtube.com/watch?v=y7Pa-9pa0nA</t>
         </is>
       </c>
       <c r="G90" t="n">
@@ -3058,26 +3058,26 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>yug2bzZrDvE</t>
+          <t>3uWDh396l-4</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>Kura (Auvergne-Rhône-Alpes) - Yanis Bennettayeb</t>
+          <t>NamCours (Ile-de-France) - Barthélémy Lorimpo  Namtchougli</t>
         </is>
       </c>
       <c r="C91" s="2" t="n">
-        <v>45732.61653935185</v>
+        <v>45731.750625</v>
       </c>
       <c r="D91" t="n">
-        <v>215</v>
+        <v>61</v>
       </c>
       <c r="E91" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=yug2bzZrDvE</t>
+          <t>https://www.youtube.com/watch?v=3uWDh396l-4</t>
         </is>
       </c>
       <c r="G91" t="n">
@@ -3087,26 +3087,26 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>_kQb_8aH0iM</t>
+          <t>ZqZYH3rExww</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>SEBLIOTECA™ (Ile de France) - Pierre Jean Sébirot</t>
+          <t>Tré D'union (Outre mer) - Jehanne Lemaud</t>
         </is>
       </c>
       <c r="C92" s="2" t="n">
-        <v>45731.71615740741</v>
+        <v>45731.691875</v>
       </c>
       <c r="D92" t="n">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="E92" t="n">
         <v>4</v>
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=_kQb_8aH0iM</t>
+          <t>https://www.youtube.com/watch?v=ZqZYH3rExww</t>
         </is>
       </c>
       <c r="G92" t="n">
@@ -3116,26 +3116,26 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>3cjVlniXX3I</t>
+          <t>yug2bzZrDvE</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>Epsilone (Auvergne-Rhône-Alpes) - Adrien Deroudille</t>
+          <t>Kura (Auvergne-Rhône-Alpes) - Yanis Bennettayeb</t>
         </is>
       </c>
       <c r="C93" s="2" t="n">
-        <v>45732.58</v>
+        <v>45732.61653935185</v>
       </c>
       <c r="D93" t="n">
-        <v>116</v>
+        <v>223</v>
       </c>
       <c r="E93" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=3cjVlniXX3I</t>
+          <t>https://www.youtube.com/watch?v=yug2bzZrDvE</t>
         </is>
       </c>
       <c r="G93" t="n">
@@ -3145,26 +3145,26 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>3uWDh396l-4</t>
+          <t>3cjVlniXX3I</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>NamCours (Ile-de-France) - Barthélémy Lorimpo  Namtchougli</t>
+          <t>Epsilone (Auvergne-Rhône-Alpes) - Adrien Deroudille</t>
         </is>
       </c>
       <c r="C94" s="2" t="n">
-        <v>45731.750625</v>
+        <v>45732.58</v>
       </c>
       <c r="D94" t="n">
-        <v>56</v>
+        <v>124</v>
       </c>
       <c r="E94" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=3uWDh396l-4</t>
+          <t>https://www.youtube.com/watch?v=3cjVlniXX3I</t>
         </is>
       </c>
       <c r="G94" t="n">
@@ -3174,26 +3174,26 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>IIV-MZacaBo</t>
+          <t>_kQb_8aH0iM</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>HAPPFLY (Ile-de-France) - Rubine Koukounda</t>
+          <t>SEBLIOTECA™ (Ile de France) - Pierre Jean Sébirot</t>
         </is>
       </c>
       <c r="C95" s="2" t="n">
-        <v>45731.73498842592</v>
+        <v>45731.71615740741</v>
       </c>
       <c r="D95" t="n">
-        <v>63</v>
+        <v>77</v>
       </c>
       <c r="E95" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=IIV-MZacaBo</t>
+          <t>https://www.youtube.com/watch?v=_kQb_8aH0iM</t>
         </is>
       </c>
       <c r="G95" t="n">
@@ -3203,26 +3203,26 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>vfuG8n-K5QM</t>
+          <t>Pswf5Z2YWS0</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>Studapp (Grand Est) - Beni Biantuadi</t>
+          <t>The meal (Ile de France) - Amadou Diallo</t>
         </is>
       </c>
       <c r="C96" s="2" t="n">
-        <v>45731.73611111111</v>
+        <v>45731.70921296296</v>
       </c>
       <c r="D96" t="n">
-        <v>71</v>
+        <v>49</v>
       </c>
       <c r="E96" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=vfuG8n-K5QM</t>
+          <t>https://www.youtube.com/watch?v=Pswf5Z2YWS0</t>
         </is>
       </c>
       <c r="G96" t="n">
@@ -3232,26 +3232,26 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>ZqZYH3rExww</t>
+          <t>vfuG8n-K5QM</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>Tré D'union (Outre mer) - Jehanne Lemaud</t>
+          <t>Studapp (Grand Est) - Beni Biantuadi</t>
         </is>
       </c>
       <c r="C97" s="2" t="n">
-        <v>45731.691875</v>
+        <v>45731.73611111111</v>
       </c>
       <c r="D97" t="n">
-        <v>52</v>
+        <v>75</v>
       </c>
       <c r="E97" t="n">
         <v>3</v>
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=ZqZYH3rExww</t>
+          <t>https://www.youtube.com/watch?v=vfuG8n-K5QM</t>
         </is>
       </c>
       <c r="G97" t="n">
@@ -3261,26 +3261,26 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>Pswf5Z2YWS0</t>
+          <t>IIV-MZacaBo</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>The meal (Ile de France) - Amadou Diallo</t>
+          <t>HAPPFLY (Ile-de-France) - Rubine Koukounda</t>
         </is>
       </c>
       <c r="C98" s="2" t="n">
-        <v>45731.70921296296</v>
+        <v>45731.73498842592</v>
       </c>
       <c r="D98" t="n">
-        <v>46</v>
+        <v>67</v>
       </c>
       <c r="E98" t="n">
         <v>3</v>
       </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=Pswf5Z2YWS0</t>
+          <t>https://www.youtube.com/watch?v=IIV-MZacaBo</t>
         </is>
       </c>
       <c r="G98" t="n">
@@ -3302,7 +3302,7 @@
         <v>45731.77209490741</v>
       </c>
       <c r="D99" t="n">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="E99" t="n">
         <v>3</v>
@@ -3319,26 +3319,26 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>uc7Ly_Dl5j4</t>
+          <t>hehjpvRhXL0</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>La floqueuse (Bretagne) - Benoit Pacaud</t>
+          <t>Eou! (Provence-Alpes-Côte d'Azur) - Clarisse Dureuil</t>
         </is>
       </c>
       <c r="C100" s="2" t="n">
-        <v>45731.70641203703</v>
+        <v>45735.62369212963</v>
       </c>
       <c r="D100" t="n">
-        <v>49</v>
+        <v>118</v>
       </c>
       <c r="E100" t="n">
         <v>2</v>
       </c>
       <c r="F100" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=uc7Ly_Dl5j4</t>
+          <t>https://www.youtube.com/watch?v=hehjpvRhXL0</t>
         </is>
       </c>
       <c r="G100" t="n">
@@ -3360,7 +3360,7 @@
         <v>45731.68236111111</v>
       </c>
       <c r="D101" t="n">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E101" t="n">
         <v>2</v>
@@ -3377,26 +3377,26 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>ufcXCCBjCwg</t>
+          <t>-P8bx4QGOsQ</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>MaeDecoo (Centre-Val de Loire) - Maëline Degas</t>
+          <t>Wolf ID (Sud) - Quentin</t>
         </is>
       </c>
       <c r="C102" s="2" t="n">
-        <v>45731.71391203703</v>
+        <v>45731.70244212963</v>
       </c>
       <c r="D102" t="n">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E102" t="n">
         <v>2</v>
       </c>
       <c r="F102" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=ufcXCCBjCwg</t>
+          <t>https://www.youtube.com/watch?v=-P8bx4QGOsQ</t>
         </is>
       </c>
       <c r="G102" t="n">
@@ -3418,10 +3418,10 @@
         <v>45731.74592592593</v>
       </c>
       <c r="D103" t="n">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="E103" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F103" t="inlineStr">
         <is>
@@ -3435,26 +3435,26 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>kaKDgZa1Ddo</t>
+          <t>2XGhNEQQyzw</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>Hunt Me (Sud) - Clara Meyer</t>
+          <t>LOOP (Pays de la Loire) - Erwan Boudaud</t>
         </is>
       </c>
       <c r="C104" s="2" t="n">
-        <v>45731.74121527778</v>
+        <v>45731.74306712963</v>
       </c>
       <c r="D104" t="n">
         <v>81</v>
       </c>
       <c r="E104" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F104" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=kaKDgZa1Ddo</t>
+          <t>https://www.youtube.com/watch?v=2XGhNEQQyzw</t>
         </is>
       </c>
       <c r="G104" t="n">
@@ -3476,10 +3476,10 @@
         <v>45731.75240740741</v>
       </c>
       <c r="D105" t="n">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="E105" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F105" t="inlineStr">
         <is>
@@ -3493,26 +3493,26 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>VdcRMnF6dpk</t>
+          <t>0HAGXiq9Uv8</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>Supermamas (Auvergne Rhônes Alpes) - Lou Pedersen</t>
+          <t>Ecogrind (Hauts de France) - Alban Crepel</t>
         </is>
       </c>
       <c r="C106" s="2" t="n">
-        <v>45731.75023148148</v>
+        <v>45731.76128472222</v>
       </c>
       <c r="D106" t="n">
-        <v>80</v>
+        <v>109</v>
       </c>
       <c r="E106" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F106" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=VdcRMnF6dpk</t>
+          <t>https://www.youtube.com/watch?v=0HAGXiq9Uv8</t>
         </is>
       </c>
       <c r="G106" t="n">
@@ -3522,26 +3522,26 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>hehjpvRhXL0</t>
+          <t>uc7Ly_Dl5j4</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>Eou! (Provence-Alpes-Côte d'Azur) - Clarisse Dureuil</t>
+          <t>La floqueuse (Bretagne) - Benoit Pacaud</t>
         </is>
       </c>
       <c r="C107" s="2" t="n">
-        <v>45735.62369212963</v>
+        <v>45731.70641203703</v>
       </c>
       <c r="D107" t="n">
-        <v>89</v>
+        <v>51</v>
       </c>
       <c r="E107" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F107" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=hehjpvRhXL0</t>
+          <t>https://www.youtube.com/watch?v=uc7Ly_Dl5j4</t>
         </is>
       </c>
       <c r="G107" t="n">
@@ -3551,26 +3551,26 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>2XGhNEQQyzw</t>
+          <t>ufcXCCBjCwg</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>LOOP (Pays de la Loire) - Erwan Boudaud</t>
+          <t>MaeDecoo (Centre-Val de Loire) - Maëline Degas</t>
         </is>
       </c>
       <c r="C108" s="2" t="n">
-        <v>45731.74306712963</v>
+        <v>45731.71391203703</v>
       </c>
       <c r="D108" t="n">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="E108" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F108" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=2XGhNEQQyzw</t>
+          <t>https://www.youtube.com/watch?v=ufcXCCBjCwg</t>
         </is>
       </c>
       <c r="G108" t="n">
@@ -3580,26 +3580,26 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>-P8bx4QGOsQ</t>
+          <t>6HjyPtMgRZY</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>Wolf ID (Sud) - Quentin</t>
+          <t>Code Citron (Ile-de-France) - Marie Auger</t>
         </is>
       </c>
       <c r="C109" s="2" t="n">
-        <v>45731.70244212963</v>
+        <v>45731.74876157408</v>
       </c>
       <c r="D109" t="n">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="E109" t="n">
         <v>1</v>
       </c>
       <c r="F109" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=-P8bx4QGOsQ</t>
+          <t>https://www.youtube.com/watch?v=6HjyPtMgRZY</t>
         </is>
       </c>
       <c r="G109" t="n">
@@ -3609,26 +3609,26 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>h6zIParalUQ</t>
+          <t>VdcRMnF6dpk</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>YFCEO (Ile-de-France) - Antonin Creignou</t>
+          <t>Supermamas (Auvergne Rhônes Alpes) - Lou Pedersen</t>
         </is>
       </c>
       <c r="C110" s="2" t="n">
-        <v>45731.70796296297</v>
+        <v>45731.75023148148</v>
       </c>
       <c r="D110" t="n">
-        <v>58</v>
+        <v>85</v>
       </c>
       <c r="E110" t="n">
         <v>1</v>
       </c>
       <c r="F110" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=h6zIParalUQ</t>
+          <t>https://www.youtube.com/watch?v=VdcRMnF6dpk</t>
         </is>
       </c>
       <c r="G110" t="n">
@@ -3638,26 +3638,26 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>HRo-IYGI2TY</t>
+          <t>xoZfR4nY2yc</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>Luxigene (Ile de France) - Chrystian Wilk</t>
+          <t>Aoz Sportswear  (Ile-de-France) - Angèle Tréhin</t>
         </is>
       </c>
       <c r="C111" s="2" t="n">
-        <v>45731.70099537037</v>
+        <v>45731.74120370371</v>
       </c>
       <c r="D111" t="n">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E111" t="n">
         <v>1</v>
       </c>
       <c r="F111" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=HRo-IYGI2TY</t>
+          <t>https://www.youtube.com/watch?v=xoZfR4nY2yc</t>
         </is>
       </c>
       <c r="G111" t="n">
@@ -3667,26 +3667,26 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>0HAGXiq9Uv8</t>
+          <t>bqODIDOHbNc</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>Ecogrind (Hauts de France) - Alban Crepel</t>
+          <t>House of Sparks (Auvergne-Rhône-Alpes) -  Gwenaëlle Yau Chun Wan</t>
         </is>
       </c>
       <c r="C112" s="2" t="n">
-        <v>45731.76128472222</v>
+        <v>45731.731875</v>
       </c>
       <c r="D112" t="n">
-        <v>100</v>
+        <v>46</v>
       </c>
       <c r="E112" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F112" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=0HAGXiq9Uv8</t>
+          <t>https://www.youtube.com/watch?v=bqODIDOHbNc</t>
         </is>
       </c>
       <c r="G112" t="n">
@@ -3696,26 +3696,26 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>6HjyPtMgRZY</t>
+          <t>kaKDgZa1Ddo</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>Code Citron (Ile-de-France) - Marie Auger</t>
+          <t>Hunt Me (Sud) - Clara Meyer</t>
         </is>
       </c>
       <c r="C113" s="2" t="n">
-        <v>45731.74876157408</v>
+        <v>45731.74121527778</v>
       </c>
       <c r="D113" t="n">
-        <v>59</v>
+        <v>89</v>
       </c>
       <c r="E113" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F113" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=6HjyPtMgRZY</t>
+          <t>https://www.youtube.com/watch?v=kaKDgZa1Ddo</t>
         </is>
       </c>
       <c r="G113" t="n">
@@ -3725,26 +3725,26 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>CjjWiohya8A</t>
+          <t>h6zIParalUQ</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>BUZU (Ile-de-France) - Sacha Boosz</t>
+          <t>YFCEO (Ile-de-France) - Antonin Creignou</t>
         </is>
       </c>
       <c r="C114" s="2" t="n">
-        <v>45731.71998842592</v>
+        <v>45731.70796296297</v>
       </c>
       <c r="D114" t="n">
-        <v>101</v>
+        <v>60</v>
       </c>
       <c r="E114" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F114" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=CjjWiohya8A</t>
+          <t>https://www.youtube.com/watch?v=h6zIParalUQ</t>
         </is>
       </c>
       <c r="G114" t="n">
@@ -3754,26 +3754,26 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>xoZfR4nY2yc</t>
+          <t>HRo-IYGI2TY</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>Aoz Sportswear  (Ile-de-France) - Angèle Tréhin</t>
+          <t>Luxigene (Ile de France) - Chrystian Wilk</t>
         </is>
       </c>
       <c r="C115" s="2" t="n">
-        <v>45731.74120370371</v>
+        <v>45731.70099537037</v>
       </c>
       <c r="D115" t="n">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="E115" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F115" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=xoZfR4nY2yc</t>
+          <t>https://www.youtube.com/watch?v=HRo-IYGI2TY</t>
         </is>
       </c>
       <c r="G115" t="n">
@@ -3783,26 +3783,26 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>bqODIDOHbNc</t>
+          <t>CjjWiohya8A</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>House of Sparks (Auvergne-Rhône-Alpes) -  Gwenaëlle Yau Chun Wan</t>
+          <t>BUZU (Ile-de-France) - Sacha Boosz</t>
         </is>
       </c>
       <c r="C116" s="2" t="n">
-        <v>45731.731875</v>
+        <v>45731.71998842592</v>
       </c>
       <c r="D116" t="n">
-        <v>43</v>
+        <v>104</v>
       </c>
       <c r="E116" t="n">
         <v>0</v>
       </c>
       <c r="F116" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=bqODIDOHbNc</t>
+          <t>https://www.youtube.com/watch?v=CjjWiohya8A</t>
         </is>
       </c>
       <c r="G116" t="n">

</xml_diff>

<commit_message>
🔄 Mise à jour auto des fichiers depuis Drive
</commit_message>
<xml_diff>
--- a/classement_youtube.xlsx
+++ b/classement_youtube.xlsx
@@ -489,7 +489,7 @@
         <v>45731.75537037037</v>
       </c>
       <c r="D2" t="n">
-        <v>6312</v>
+        <v>6314</v>
       </c>
       <c r="E2" t="n">
         <v>5635</v>
@@ -518,10 +518,10 @@
         <v>45731.65984953703</v>
       </c>
       <c r="D3" t="n">
-        <v>4167</v>
+        <v>4177</v>
       </c>
       <c r="E3" t="n">
-        <v>1421</v>
+        <v>1420</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -535,26 +535,26 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>mEzVlJuxkX8</t>
+          <t>Ol91C4pV3kA</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Immonator (Ile de France) - Andreas Gauthier</t>
+          <t>Les Trésors d'Ulysse (Hauts de France) - Gaëlle Vasse</t>
         </is>
       </c>
       <c r="C4" s="2" t="n">
-        <v>45731.65702546296</v>
+        <v>45731.68711805555</v>
       </c>
       <c r="D4" t="n">
-        <v>3367</v>
+        <v>2340</v>
       </c>
       <c r="E4" t="n">
-        <v>1302</v>
+        <v>1355</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=mEzVlJuxkX8</t>
+          <t>https://www.youtube.com/watch?v=Ol91C4pV3kA</t>
         </is>
       </c>
       <c r="G4" t="n">
@@ -564,26 +564,26 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>5FjGLct9MQk</t>
+          <t>mEzVlJuxkX8</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>LuminyShop (Sud) - Michael Jeanmonod</t>
+          <t>Immonator (Ile de France) - Andreas Gauthier</t>
         </is>
       </c>
       <c r="C5" s="2" t="n">
-        <v>45731.67113425926</v>
+        <v>45731.65702546296</v>
       </c>
       <c r="D5" t="n">
-        <v>3507</v>
+        <v>3369</v>
       </c>
       <c r="E5" t="n">
-        <v>1225</v>
+        <v>1303</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=5FjGLct9MQk</t>
+          <t>https://www.youtube.com/watch?v=mEzVlJuxkX8</t>
         </is>
       </c>
       <c r="G5" t="n">
@@ -593,26 +593,26 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>hoA6ZAlniU4</t>
+          <t>5FjGLct9MQk</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Van&amp;Camp (Occitanie) - Célia Lauret</t>
+          <t>LuminyShop (Sud) - Michael Jeanmonod</t>
         </is>
       </c>
       <c r="C6" s="2" t="n">
-        <v>45731.73765046296</v>
+        <v>45731.67113425926</v>
       </c>
       <c r="D6" t="n">
-        <v>2257</v>
+        <v>3547</v>
       </c>
       <c r="E6" t="n">
-        <v>1192</v>
+        <v>1233</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=hoA6ZAlniU4</t>
+          <t>https://www.youtube.com/watch?v=5FjGLct9MQk</t>
         </is>
       </c>
       <c r="G6" t="n">
@@ -622,26 +622,26 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>rFiK84r-V5I</t>
+          <t>hoA6ZAlniU4</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>NeoSense (Ile de France) - Pierrick Legrand</t>
+          <t>Van&amp;Camp (Occitanie) - Célia Lauret</t>
         </is>
       </c>
       <c r="C7" s="2" t="n">
-        <v>45731.69415509259</v>
+        <v>45731.73765046296</v>
       </c>
       <c r="D7" t="n">
-        <v>5097</v>
+        <v>2257</v>
       </c>
       <c r="E7" t="n">
-        <v>1117</v>
+        <v>1192</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=rFiK84r-V5I</t>
+          <t>https://www.youtube.com/watch?v=hoA6ZAlniU4</t>
         </is>
       </c>
       <c r="G7" t="n">
@@ -651,26 +651,26 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>_bc5qhnNgJM</t>
+          <t>rFiK84r-V5I</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>LC (Hauts de France) - Brice Moscatello</t>
+          <t>NeoSense (Ile de France) - Pierrick Legrand</t>
         </is>
       </c>
       <c r="C8" s="2" t="n">
-        <v>45731.70519675926</v>
+        <v>45731.69415509259</v>
       </c>
       <c r="D8" t="n">
-        <v>1447</v>
+        <v>5098</v>
       </c>
       <c r="E8" t="n">
-        <v>1036</v>
+        <v>1118</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=_bc5qhnNgJM</t>
+          <t>https://www.youtube.com/watch?v=rFiK84r-V5I</t>
         </is>
       </c>
       <c r="G8" t="n">
@@ -680,26 +680,26 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>cW2UNYLYPBI</t>
+          <t>_bc5qhnNgJM</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>HKN Corporation (Grand Est) - Quentin Hamza</t>
+          <t>LC (Hauts de France) - Brice Moscatello</t>
         </is>
       </c>
       <c r="C9" s="2" t="n">
-        <v>45731.78427083333</v>
+        <v>45731.70519675926</v>
       </c>
       <c r="D9" t="n">
-        <v>2881</v>
+        <v>1459</v>
       </c>
       <c r="E9" t="n">
-        <v>899</v>
+        <v>1042</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=cW2UNYLYPBI</t>
+          <t>https://www.youtube.com/watch?v=_bc5qhnNgJM</t>
         </is>
       </c>
       <c r="G9" t="n">
@@ -709,26 +709,26 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>j0s2-clRSTs</t>
+          <t>cW2UNYLYPBI</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>LeadLink (Bourgogne-Franche-Comté) -  Shana Husejnovic</t>
+          <t>HKN Corporation (Grand Est) - Quentin Hamza</t>
         </is>
       </c>
       <c r="C10" s="2" t="n">
-        <v>45731.74269675926</v>
+        <v>45731.78427083333</v>
       </c>
       <c r="D10" t="n">
-        <v>2738</v>
+        <v>2999</v>
       </c>
       <c r="E10" t="n">
-        <v>762</v>
+        <v>957</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=j0s2-clRSTs</t>
+          <t>https://www.youtube.com/watch?v=cW2UNYLYPBI</t>
         </is>
       </c>
       <c r="G10" t="n">
@@ -738,26 +738,26 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Ol91C4pV3kA</t>
+          <t>j0s2-clRSTs</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Les Trésors d'Ulysse (Hauts de France) - Gaëlle Vasse</t>
+          <t>LeadLink (Bourgogne-Franche-Comté) -  Shana Husejnovic</t>
         </is>
       </c>
       <c r="C11" s="2" t="n">
-        <v>45731.68711805555</v>
+        <v>45731.74269675926</v>
       </c>
       <c r="D11" t="n">
-        <v>2273</v>
+        <v>2744</v>
       </c>
       <c r="E11" t="n">
-        <v>731</v>
+        <v>762</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=Ol91C4pV3kA</t>
+          <t>https://www.youtube.com/watch?v=j0s2-clRSTs</t>
         </is>
       </c>
       <c r="G11" t="n">
@@ -779,10 +779,10 @@
         <v>45733.37125</v>
       </c>
       <c r="D12" t="n">
-        <v>1726</v>
+        <v>1758</v>
       </c>
       <c r="E12" t="n">
-        <v>708</v>
+        <v>717</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
@@ -808,7 +808,7 @@
         <v>45731.70387731482</v>
       </c>
       <c r="D13" t="n">
-        <v>2545</v>
+        <v>2550</v>
       </c>
       <c r="E13" t="n">
         <v>688</v>
@@ -837,10 +837,10 @@
         <v>45731.70635416666</v>
       </c>
       <c r="D14" t="n">
-        <v>2731</v>
+        <v>2751</v>
       </c>
       <c r="E14" t="n">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
@@ -866,10 +866,10 @@
         <v>45731.7728587963</v>
       </c>
       <c r="D15" t="n">
-        <v>3026</v>
+        <v>3038</v>
       </c>
       <c r="E15" t="n">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
@@ -895,10 +895,10 @@
         <v>45731.71851851852</v>
       </c>
       <c r="D16" t="n">
-        <v>2463</v>
+        <v>2468</v>
       </c>
       <c r="E16" t="n">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
@@ -924,7 +924,7 @@
         <v>45731.68974537037</v>
       </c>
       <c r="D17" t="n">
-        <v>1730</v>
+        <v>1771</v>
       </c>
       <c r="E17" t="n">
         <v>453</v>
@@ -982,10 +982,10 @@
         <v>45731.71129629629</v>
       </c>
       <c r="D19" t="n">
-        <v>2441</v>
+        <v>2458</v>
       </c>
       <c r="E19" t="n">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
@@ -1011,7 +1011,7 @@
         <v>45731.72594907408</v>
       </c>
       <c r="D20" t="n">
-        <v>1479</v>
+        <v>1483</v>
       </c>
       <c r="E20" t="n">
         <v>365</v>
@@ -1057,26 +1057,26 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>zbFwgdhJjC8</t>
+          <t>cpP4q3pS1Vc</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>PreSkinS (Auvergne Rhône Alpes) - Hugo Cocquet</t>
+          <t>Sam J (Occitanie) - Samantha VOLCY</t>
         </is>
       </c>
       <c r="C22" s="2" t="n">
-        <v>45731.66652777778</v>
+        <v>45731.67795138889</v>
       </c>
       <c r="D22" t="n">
-        <v>1218</v>
+        <v>1310</v>
       </c>
       <c r="E22" t="n">
         <v>328</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=zbFwgdhJjC8</t>
+          <t>https://www.youtube.com/watch?v=cpP4q3pS1Vc</t>
         </is>
       </c>
       <c r="G22" t="n">
@@ -1086,26 +1086,26 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>cpP4q3pS1Vc</t>
+          <t>zbFwgdhJjC8</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Sam J (Occitanie) - Samantha VOLCY</t>
+          <t>PreSkinS (Auvergne Rhône Alpes) - Hugo Cocquet</t>
         </is>
       </c>
       <c r="C23" s="2" t="n">
-        <v>45731.67795138889</v>
+        <v>45731.66652777778</v>
       </c>
       <c r="D23" t="n">
-        <v>1308</v>
+        <v>1218</v>
       </c>
       <c r="E23" t="n">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=cpP4q3pS1Vc</t>
+          <t>https://www.youtube.com/watch?v=zbFwgdhJjC8</t>
         </is>
       </c>
       <c r="G23" t="n">
@@ -1127,7 +1127,7 @@
         <v>45731.74208333333</v>
       </c>
       <c r="D24" t="n">
-        <v>2019</v>
+        <v>2021</v>
       </c>
       <c r="E24" t="n">
         <v>305</v>
@@ -1156,7 +1156,7 @@
         <v>45731.746875</v>
       </c>
       <c r="D25" t="n">
-        <v>1121</v>
+        <v>1122</v>
       </c>
       <c r="E25" t="n">
         <v>285</v>
@@ -1214,10 +1214,10 @@
         <v>45731.66978009259</v>
       </c>
       <c r="D27" t="n">
-        <v>1051</v>
+        <v>1053</v>
       </c>
       <c r="E27" t="n">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>
@@ -1243,10 +1243,10 @@
         <v>45732.61858796296</v>
       </c>
       <c r="D28" t="n">
-        <v>1083</v>
+        <v>1087</v>
       </c>
       <c r="E28" t="n">
-        <v>242</v>
+        <v>247</v>
       </c>
       <c r="F28" t="inlineStr">
         <is>
@@ -1272,7 +1272,7 @@
         <v>45731.71417824074</v>
       </c>
       <c r="D29" t="n">
-        <v>1261</v>
+        <v>1262</v>
       </c>
       <c r="E29" t="n">
         <v>242</v>
@@ -1301,10 +1301,10 @@
         <v>45732.61717592592</v>
       </c>
       <c r="D30" t="n">
-        <v>1653</v>
+        <v>1657</v>
       </c>
       <c r="E30" t="n">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F30" t="inlineStr">
         <is>
@@ -1330,10 +1330,10 @@
         <v>45731.74027777778</v>
       </c>
       <c r="D31" t="n">
-        <v>1548</v>
+        <v>1558</v>
       </c>
       <c r="E31" t="n">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="F31" t="inlineStr">
         <is>
@@ -1388,7 +1388,7 @@
         <v>45731.69851851852</v>
       </c>
       <c r="D33" t="n">
-        <v>890</v>
+        <v>891</v>
       </c>
       <c r="E33" t="n">
         <v>196</v>
@@ -1417,7 +1417,7 @@
         <v>45731.77814814815</v>
       </c>
       <c r="D34" t="n">
-        <v>871</v>
+        <v>873</v>
       </c>
       <c r="E34" t="n">
         <v>185</v>
@@ -1434,26 +1434,26 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>ak7VnMRovWc</t>
+          <t>i9e-beHIxJo</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Primaire (Grand Est) - Lucie Le May</t>
+          <t>Handépassement (Ile de France) - Myriam Hakem</t>
         </is>
       </c>
       <c r="C35" s="2" t="n">
-        <v>45731.7528587963</v>
+        <v>45731.67952546296</v>
       </c>
       <c r="D35" t="n">
-        <v>869</v>
+        <v>982</v>
       </c>
       <c r="E35" t="n">
-        <v>168</v>
+        <v>176</v>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=ak7VnMRovWc</t>
+          <t>https://www.youtube.com/watch?v=i9e-beHIxJo</t>
         </is>
       </c>
       <c r="G35" t="n">
@@ -1463,26 +1463,26 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>w4_H7lnDxHw</t>
+          <t>ak7VnMRovWc</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Revisité Ile-de-France) - Anne Gulino</t>
+          <t>Primaire (Grand Est) - Lucie Le May</t>
         </is>
       </c>
       <c r="C36" s="2" t="n">
-        <v>45731.71700231481</v>
+        <v>45731.7528587963</v>
       </c>
       <c r="D36" t="n">
-        <v>582</v>
+        <v>869</v>
       </c>
       <c r="E36" t="n">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=w4_H7lnDxHw</t>
+          <t>https://www.youtube.com/watch?v=ak7VnMRovWc</t>
         </is>
       </c>
       <c r="G36" t="n">
@@ -1492,26 +1492,26 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Lgb9olWKkBg</t>
+          <t>w4_H7lnDxHw</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Ride Enjoy (Pays de la Loire) - Léo Gentilhomme</t>
+          <t>Revisité Ile-de-France) - Anne Gulino</t>
         </is>
       </c>
       <c r="C37" s="2" t="n">
-        <v>45731.69020833333</v>
+        <v>45731.71700231481</v>
       </c>
       <c r="D37" t="n">
-        <v>1130</v>
+        <v>582</v>
       </c>
       <c r="E37" t="n">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=Lgb9olWKkBg</t>
+          <t>https://www.youtube.com/watch?v=w4_H7lnDxHw</t>
         </is>
       </c>
       <c r="G37" t="n">
@@ -1521,26 +1521,26 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>85Ng9KHHQPo</t>
+          <t>Lgb9olWKkBg</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Pâtatra (Hauts-de-France) - Erwan Goussot</t>
+          <t>Ride Enjoy (Pays de la Loire) - Léo Gentilhomme</t>
         </is>
       </c>
       <c r="C38" s="2" t="n">
-        <v>45731.70513888889</v>
+        <v>45731.69020833333</v>
       </c>
       <c r="D38" t="n">
-        <v>481</v>
+        <v>1133</v>
       </c>
       <c r="E38" t="n">
-        <v>150</v>
+        <v>162</v>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=85Ng9KHHQPo</t>
+          <t>https://www.youtube.com/watch?v=Lgb9olWKkBg</t>
         </is>
       </c>
       <c r="G38" t="n">
@@ -1550,26 +1550,26 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>d0WaiIGQI_A</t>
+          <t>85Ng9KHHQPo</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Cellule Rouge (Nouvelle Aquitaine) -  Benjamin Leroy</t>
+          <t>Pâtatra (Hauts-de-France) - Erwan Goussot</t>
         </is>
       </c>
       <c r="C39" s="2" t="n">
-        <v>45731.73831018519</v>
+        <v>45731.70513888889</v>
       </c>
       <c r="D39" t="n">
-        <v>832</v>
+        <v>481</v>
       </c>
       <c r="E39" t="n">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=d0WaiIGQI_A</t>
+          <t>https://www.youtube.com/watch?v=85Ng9KHHQPo</t>
         </is>
       </c>
       <c r="G39" t="n">
@@ -1608,26 +1608,26 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>i9e-beHIxJo</t>
+          <t>d0WaiIGQI_A</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Handépassement (Ile de France) - Myriam Hakem</t>
+          <t>Cellule Rouge (Nouvelle Aquitaine) -  Benjamin Leroy</t>
         </is>
       </c>
       <c r="C41" s="2" t="n">
-        <v>45731.67952546296</v>
+        <v>45731.73831018519</v>
       </c>
       <c r="D41" t="n">
-        <v>966</v>
+        <v>837</v>
       </c>
       <c r="E41" t="n">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=i9e-beHIxJo</t>
+          <t>https://www.youtube.com/watch?v=d0WaiIGQI_A</t>
         </is>
       </c>
       <c r="G41" t="n">
@@ -1649,7 +1649,7 @@
         <v>45731.66284722222</v>
       </c>
       <c r="D42" t="n">
-        <v>982</v>
+        <v>983</v>
       </c>
       <c r="E42" t="n">
         <v>146</v>
@@ -1678,10 +1678,10 @@
         <v>45731.72136574074</v>
       </c>
       <c r="D43" t="n">
-        <v>364</v>
+        <v>368</v>
       </c>
       <c r="E43" t="n">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="F43" t="inlineStr">
         <is>
@@ -1707,7 +1707,7 @@
         <v>45732.65084490741</v>
       </c>
       <c r="D44" t="n">
-        <v>661</v>
+        <v>663</v>
       </c>
       <c r="E44" t="n">
         <v>133</v>
@@ -1736,7 +1736,7 @@
         <v>45731.65853009259</v>
       </c>
       <c r="D45" t="n">
-        <v>803</v>
+        <v>805</v>
       </c>
       <c r="E45" t="n">
         <v>116</v>
@@ -1765,7 +1765,7 @@
         <v>45731.76277777777</v>
       </c>
       <c r="D46" t="n">
-        <v>1248</v>
+        <v>1251</v>
       </c>
       <c r="E46" t="n">
         <v>113</v>
@@ -1794,7 +1794,7 @@
         <v>45733.4946875</v>
       </c>
       <c r="D47" t="n">
-        <v>1244</v>
+        <v>1247</v>
       </c>
       <c r="E47" t="n">
         <v>108</v>
@@ -1823,7 +1823,7 @@
         <v>45731.69076388889</v>
       </c>
       <c r="D48" t="n">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="E48" t="n">
         <v>107</v>
@@ -1852,7 +1852,7 @@
         <v>45732.61524305555</v>
       </c>
       <c r="D49" t="n">
-        <v>846</v>
+        <v>849</v>
       </c>
       <c r="E49" t="n">
         <v>91</v>
@@ -1881,7 +1881,7 @@
         <v>45732.61957175926</v>
       </c>
       <c r="D50" t="n">
-        <v>617</v>
+        <v>620</v>
       </c>
       <c r="E50" t="n">
         <v>90</v>
@@ -1910,7 +1910,7 @@
         <v>45731.74450231482</v>
       </c>
       <c r="D51" t="n">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="E51" t="n">
         <v>86</v>
@@ -1939,10 +1939,10 @@
         <v>45731.73282407408</v>
       </c>
       <c r="D52" t="n">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="E52" t="n">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="F52" t="inlineStr">
         <is>
@@ -2026,7 +2026,7 @@
         <v>45731.69967592593</v>
       </c>
       <c r="D55" t="n">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="E55" t="n">
         <v>67</v>
@@ -2113,7 +2113,7 @@
         <v>45731.75940972222</v>
       </c>
       <c r="D58" t="n">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="E58" t="n">
         <v>53</v>
@@ -2142,7 +2142,7 @@
         <v>45732.56851851852</v>
       </c>
       <c r="D59" t="n">
-        <v>523</v>
+        <v>525</v>
       </c>
       <c r="E59" t="n">
         <v>52</v>
@@ -2171,7 +2171,7 @@
         <v>45731.73631944445</v>
       </c>
       <c r="D60" t="n">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="E60" t="n">
         <v>52</v>
@@ -2200,7 +2200,7 @@
         <v>45731.74563657407</v>
       </c>
       <c r="D61" t="n">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="E61" t="n">
         <v>52</v>
@@ -2258,7 +2258,7 @@
         <v>45734.61689814815</v>
       </c>
       <c r="D63" t="n">
-        <v>455</v>
+        <v>461</v>
       </c>
       <c r="E63" t="n">
         <v>47</v>
@@ -2287,7 +2287,7 @@
         <v>45731.66840277778</v>
       </c>
       <c r="D64" t="n">
-        <v>920</v>
+        <v>928</v>
       </c>
       <c r="E64" t="n">
         <v>45</v>
@@ -2362,26 +2362,26 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>OVg1lgo34ng</t>
+          <t>TFryzA55HpI</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Mikoo (Provence-Alpes-Côte d’Azur) - Lucas Cuordifede</t>
+          <t>Lueurs d'antan (Bretagne) - Axelle Trouillet</t>
         </is>
       </c>
       <c r="C67" s="2" t="n">
-        <v>45732.88743055556</v>
+        <v>45732.62079861111</v>
       </c>
       <c r="D67" t="n">
-        <v>414</v>
+        <v>284</v>
       </c>
       <c r="E67" t="n">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=OVg1lgo34ng</t>
+          <t>https://www.youtube.com/watch?v=TFryzA55HpI</t>
         </is>
       </c>
       <c r="G67" t="n">
@@ -2391,26 +2391,26 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>HhN8skozWWM</t>
+          <t>OVg1lgo34ng</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Hyppalektryon (Hauts-de-France) - Elisa Douchez</t>
+          <t>Mikoo (Provence-Alpes-Côte d’Azur) - Lucas Cuordifede</t>
         </is>
       </c>
       <c r="C68" s="2" t="n">
-        <v>45731.73899305556</v>
+        <v>45732.88743055556</v>
       </c>
       <c r="D68" t="n">
-        <v>246</v>
+        <v>415</v>
       </c>
       <c r="E68" t="n">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=HhN8skozWWM</t>
+          <t>https://www.youtube.com/watch?v=OVg1lgo34ng</t>
         </is>
       </c>
       <c r="G68" t="n">
@@ -2420,26 +2420,26 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>uUnH8dwM4CE</t>
+          <t>HhN8skozWWM</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Auliviha (Ile-de-France) - Olivia Luscap</t>
+          <t>Hyppalektryon (Hauts-de-France) - Elisa Douchez</t>
         </is>
       </c>
       <c r="C69" s="2" t="n">
-        <v>45731.73412037037</v>
+        <v>45731.73899305556</v>
       </c>
       <c r="D69" t="n">
-        <v>210</v>
+        <v>246</v>
       </c>
       <c r="E69" t="n">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=uUnH8dwM4CE</t>
+          <t>https://www.youtube.com/watch?v=HhN8skozWWM</t>
         </is>
       </c>
       <c r="G69" t="n">
@@ -2449,26 +2449,26 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>TFryzA55HpI</t>
+          <t>uUnH8dwM4CE</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Lueurs d'antan (Bretagne) - Axelle Trouillet</t>
+          <t>Auliviha (Ile-de-France) - Olivia Luscap</t>
         </is>
       </c>
       <c r="C70" s="2" t="n">
-        <v>45732.62079861111</v>
+        <v>45731.73412037037</v>
       </c>
       <c r="D70" t="n">
-        <v>238</v>
+        <v>215</v>
       </c>
       <c r="E70" t="n">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=TFryzA55HpI</t>
+          <t>https://www.youtube.com/watch?v=uUnH8dwM4CE</t>
         </is>
       </c>
       <c r="G70" t="n">
@@ -2490,7 +2490,7 @@
         <v>45731.69685185186</v>
       </c>
       <c r="D71" t="n">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E71" t="n">
         <v>30</v>
@@ -2577,7 +2577,7 @@
         <v>45731.69309027777</v>
       </c>
       <c r="D74" t="n">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="E74" t="n">
         <v>22</v>
@@ -2664,7 +2664,7 @@
         <v>45732.62953703704</v>
       </c>
       <c r="D77" t="n">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="E77" t="n">
         <v>20</v>
@@ -2693,7 +2693,7 @@
         <v>45731.75690972222</v>
       </c>
       <c r="D78" t="n">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E78" t="n">
         <v>19</v>
@@ -2780,7 +2780,7 @@
         <v>45735.49681712963</v>
       </c>
       <c r="D81" t="n">
-        <v>412</v>
+        <v>417</v>
       </c>
       <c r="E81" t="n">
         <v>13</v>
@@ -2797,26 +2797,26 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>zjNk_GBOz-U</t>
+          <t>YxsHa3ivN3k</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Les Harmonieuses (Ile de France) - Elodie Te</t>
+          <t>Caelum (Occitanie) - Juan Carlos Guzman</t>
         </is>
       </c>
       <c r="C82" s="2" t="n">
-        <v>45731.7478587963</v>
+        <v>45732.57215277778</v>
       </c>
       <c r="D82" t="n">
-        <v>130</v>
+        <v>164</v>
       </c>
       <c r="E82" t="n">
         <v>12</v>
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=zjNk_GBOz-U</t>
+          <t>https://www.youtube.com/watch?v=YxsHa3ivN3k</t>
         </is>
       </c>
       <c r="G82" t="n">
@@ -2826,26 +2826,26 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>l11oYhr0tX8</t>
+          <t>zjNk_GBOz-U</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>MindCare (Ile-de-France) - Djenaba Toure</t>
+          <t>Les Harmonieuses (Ile de France) - Elodie Te</t>
         </is>
       </c>
       <c r="C83" s="2" t="n">
-        <v>45732.58172453703</v>
+        <v>45731.7478587963</v>
       </c>
       <c r="D83" t="n">
-        <v>154</v>
+        <v>130</v>
       </c>
       <c r="E83" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=l11oYhr0tX8</t>
+          <t>https://www.youtube.com/watch?v=zjNk_GBOz-U</t>
         </is>
       </c>
       <c r="G83" t="n">
@@ -2855,26 +2855,26 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>8u2qC29LxPE</t>
+          <t>l11oYhr0tX8</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>La Repousse (Grand Est) - Viktor Macé</t>
+          <t>MindCare (Ile-de-France) - Djenaba Toure</t>
         </is>
       </c>
       <c r="C84" s="2" t="n">
-        <v>45736.40002314815</v>
+        <v>45732.58172453703</v>
       </c>
       <c r="D84" t="n">
-        <v>214</v>
+        <v>158</v>
       </c>
       <c r="E84" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=8u2qC29LxPE</t>
+          <t>https://www.youtube.com/watch?v=l11oYhr0tX8</t>
         </is>
       </c>
       <c r="G84" t="n">
@@ -2884,26 +2884,26 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>R9b2eIvRYGI</t>
+          <t>8u2qC29LxPE</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Povi (Ile-de-France) - Cornelia Allagbe</t>
+          <t>La Repousse (Grand Est) - Viktor Macé</t>
         </is>
       </c>
       <c r="C85" s="2" t="n">
-        <v>45732.58274305556</v>
+        <v>45736.40002314815</v>
       </c>
       <c r="D85" t="n">
-        <v>103</v>
+        <v>217</v>
       </c>
       <c r="E85" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=R9b2eIvRYGI</t>
+          <t>https://www.youtube.com/watch?v=8u2qC29LxPE</t>
         </is>
       </c>
       <c r="G85" t="n">
@@ -2913,26 +2913,26 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>YxsHa3ivN3k</t>
+          <t>R9b2eIvRYGI</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Caelum (Occitanie) - Juan Carlos Guzman</t>
+          <t>Povi (Ile-de-France) - Cornelia Allagbe</t>
         </is>
       </c>
       <c r="C86" s="2" t="n">
-        <v>45732.57215277778</v>
+        <v>45732.58274305556</v>
       </c>
       <c r="D86" t="n">
-        <v>160</v>
+        <v>103</v>
       </c>
       <c r="E86" t="n">
         <v>9</v>
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=YxsHa3ivN3k</t>
+          <t>https://www.youtube.com/watch?v=R9b2eIvRYGI</t>
         </is>
       </c>
       <c r="G86" t="n">
@@ -2954,7 +2954,7 @@
         <v>45731.67466435185</v>
       </c>
       <c r="D87" t="n">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="E87" t="n">
         <v>7</v>
@@ -3058,26 +3058,26 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>3uWDh396l-4</t>
+          <t>3cjVlniXX3I</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>NamCours (Ile-de-France) - Barthélémy Lorimpo  Namtchougli</t>
+          <t>Epsilone (Auvergne-Rhône-Alpes) - Adrien Deroudille</t>
         </is>
       </c>
       <c r="C91" s="2" t="n">
-        <v>45731.750625</v>
+        <v>45732.58</v>
       </c>
       <c r="D91" t="n">
-        <v>61</v>
+        <v>126</v>
       </c>
       <c r="E91" t="n">
         <v>5</v>
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=3uWDh396l-4</t>
+          <t>https://www.youtube.com/watch?v=3cjVlniXX3I</t>
         </is>
       </c>
       <c r="G91" t="n">
@@ -3087,26 +3087,26 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>ZqZYH3rExww</t>
+          <t>3uWDh396l-4</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>Tré D'union (Outre mer) - Jehanne Lemaud</t>
+          <t>NamCours (Ile-de-France) - Barthélémy Lorimpo  Namtchougli</t>
         </is>
       </c>
       <c r="C92" s="2" t="n">
-        <v>45731.691875</v>
+        <v>45731.750625</v>
       </c>
       <c r="D92" t="n">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="E92" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=ZqZYH3rExww</t>
+          <t>https://www.youtube.com/watch?v=3uWDh396l-4</t>
         </is>
       </c>
       <c r="G92" t="n">
@@ -3128,7 +3128,7 @@
         <v>45732.61653935185</v>
       </c>
       <c r="D93" t="n">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="E93" t="n">
         <v>4</v>
@@ -3145,26 +3145,26 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>3cjVlniXX3I</t>
+          <t>ZqZYH3rExww</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>Epsilone (Auvergne-Rhône-Alpes) - Adrien Deroudille</t>
+          <t>Tré D'union (Outre mer) - Jehanne Lemaud</t>
         </is>
       </c>
       <c r="C94" s="2" t="n">
-        <v>45732.58</v>
+        <v>45731.691875</v>
       </c>
       <c r="D94" t="n">
-        <v>124</v>
+        <v>56</v>
       </c>
       <c r="E94" t="n">
         <v>4</v>
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=3cjVlniXX3I</t>
+          <t>https://www.youtube.com/watch?v=ZqZYH3rExww</t>
         </is>
       </c>
       <c r="G94" t="n">
@@ -3244,7 +3244,7 @@
         <v>45731.73611111111</v>
       </c>
       <c r="D97" t="n">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E97" t="n">
         <v>3</v>
@@ -3302,7 +3302,7 @@
         <v>45731.77209490741</v>
       </c>
       <c r="D99" t="n">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="E99" t="n">
         <v>3</v>
@@ -3331,7 +3331,7 @@
         <v>45735.62369212963</v>
       </c>
       <c r="D100" t="n">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="E100" t="n">
         <v>2</v>
@@ -3505,7 +3505,7 @@
         <v>45731.76128472222</v>
       </c>
       <c r="D106" t="n">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="E106" t="n">
         <v>2</v>
@@ -3534,7 +3534,7 @@
         <v>45731.70641203703</v>
       </c>
       <c r="D107" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E107" t="n">
         <v>2</v>
@@ -3592,7 +3592,7 @@
         <v>45731.74876157408</v>
       </c>
       <c r="D109" t="n">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E109" t="n">
         <v>1</v>
@@ -3679,7 +3679,7 @@
         <v>45731.731875</v>
       </c>
       <c r="D112" t="n">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E112" t="n">
         <v>1</v>
@@ -3708,7 +3708,7 @@
         <v>45731.74121527778</v>
       </c>
       <c r="D113" t="n">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E113" t="n">
         <v>1</v>

</xml_diff>